<commit_message>
add problems  and their solutions
</commit_message>
<xml_diff>
--- a/Docs/reports/Our achievements.xlsx
+++ b/Docs/reports/Our achievements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Tasks</t>
   </si>
@@ -78,19 +78,50 @@
     <t>8. Explain how to create sequence diagrams</t>
   </si>
   <si>
-    <t>−</t>
-  </si>
-  <si>
-    <t>1.Understand what SAD includes 2.Create use cases, which be description of business processes</t>
-  </si>
-  <si>
-    <t>1. Find inforfation about SAD   2.Created Use Cases</t>
-  </si>
-  <si>
-    <t>1.  Completely different understanding of what is Use Case diagrams</t>
-  </si>
-  <si>
-    <t>1. Discussion of the problem, what  Use Cases we must  do with Andrii Tymchuk</t>
+    <t>We had problems with the hard realization database  requests for reporting</t>
+  </si>
+  <si>
+    <t>We discussed with the team ER diagram and made ​​adjustments</t>
+  </si>
+  <si>
+    <t>To understand whether the Anatolii Connection Pool  is thread-safe and  multi-threaded. At first I thought that it is not thread-safe and multi-threaded.</t>
+  </si>
+  <si>
+    <t>Gradually there are various minor problems</t>
+  </si>
+  <si>
+    <t>Solving these problems is finding relevant information and clarify difficult issues with authors.</t>
+  </si>
+  <si>
+    <t>Special problems have arisen</t>
+  </si>
+  <si>
+    <t>1. Understand what SAD includes  2.Create use cases, which be description of business processes</t>
+  </si>
+  <si>
+    <t>Carefully verify all requirements and use cases</t>
+  </si>
+  <si>
+    <t>Answer the question whether all requirements we have covered with use cases</t>
+  </si>
+  <si>
+    <t>1. Find inforfation about SAD    2.Created Use Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  Completely different understanding of what is Use Case diagrams  2. Problems with descriptions  "Creating Service Order", "Review Service Order", "Creating New Circuit in System" and "Creating Service Instance" use cases </t>
+  </si>
+  <si>
+    <t>1. Discussion of the problem, what  Use Cases we must  do with curators  2.Discussion and resolve issues with the team and  curators how these processes will be implemented .</t>
+  </si>
+  <si>
+    <t>1. Problems so that the server does not return the data to the ajax query. 2. Problems to display Hart CSEDashboard  3.Purification derived table  4. Raging and pagination</t>
+  </si>
+  <si>
+    <t>1. Solving the problem is not with the server, but with the inability to retrieve data from the database. 
+2. A more detailed study of CSS, HTML, JS. All bootstrap framework.        3-4. The solution of 30%, familiarization with cursor</t>
+  </si>
+  <si>
+    <t>The fact that our ConnectionPool  is safe-thread confirmed usssng singletone pattern and the fact it is multithreaded singletone  confirmed pool setting . Find information   about singletone and ThreadLocal class.</t>
   </si>
 </sst>
 </file>
@@ -407,6 +438,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -416,26 +465,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,16 +771,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
@@ -767,7 +798,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5"/>
@@ -775,13 +806,13 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="14"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="15"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
@@ -801,111 +832,129 @@
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="18"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" ht="48.75" customHeight="1">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:4" ht="75.75" customHeight="1">
+      <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48.75" customHeight="1">
-      <c r="A9" s="14"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A10" s="14"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45.75" customHeight="1">
+      <c r="A10" s="20"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30">
-      <c r="A11" s="14"/>
+      <c r="C10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1">
+      <c r="A11" s="20"/>
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="14"/>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="75.75" customHeight="1">
+      <c r="A12" s="20"/>
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" s="14"/>
+      <c r="C12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45">
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="14"/>
+      <c r="C13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="93" customHeight="1">
+      <c r="A14" s="20"/>
       <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A15" s="15"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="17"/>
-      <c r="B17" s="20"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A18" s="18"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="5"/>
@@ -913,13 +962,13 @@
       <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A20" s="14"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A21" s="15"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -939,13 +988,13 @@
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A24" s="18"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="5"/>
@@ -953,13 +1002,13 @@
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A26" s="14"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A27" s="15"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -979,7 +1028,7 @@
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A30" s="19"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>

</xml_diff>

<commit_message>
Anna (tasks, problems, how solving problems )
</commit_message>
<xml_diff>
--- a/Docs/reports/Our achievements.xlsx
+++ b/Docs/reports/Our achievements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Tasks</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Solving these problems is finding relevant information and clarify difficult issues with authors.</t>
-  </si>
-  <si>
-    <t>Special problems have arisen</t>
   </si>
   <si>
     <t>1. Understand what SAD includes  2.Create use cases, which be description of business processes</t>
@@ -121,7 +118,13 @@
 2. A more detailed study of CSS, HTML, JS. All bootstrap framework.        3-4. The solution of 30%, familiarization with cursor</t>
   </si>
   <si>
-    <t>The fact that our ConnectionPool  is safe-thread confirmed usssng singletone pattern and the fact it is multithreaded singletone  confirmed pool setting . Find information   about singletone and ThreadLocal class.</t>
+    <t>The fact that our ConnectionPool  is safe-thread confirmed using singleton pattern and the fact it is multithreaded singleton  confirmed pool setting . Find information   about singletone and ThreadLocal class.</t>
+  </si>
+  <si>
+    <t>Find tutorials about it.</t>
+  </si>
+  <si>
+    <t>How sequence diagram to depict a link to another sequence diagram.</t>
   </si>
 </sst>
 </file>
@@ -771,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,10 +848,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48.75" customHeight="1">
@@ -857,10 +860,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45.75" customHeight="1">
@@ -869,10 +872,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" customHeight="1">
@@ -896,7 +899,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45">
@@ -917,10 +920,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30.75" customHeight="1">
@@ -929,9 +932,11 @@
         <v>19</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">

</xml_diff>